<commit_message>
House Keeping and General Analysis
</commit_message>
<xml_diff>
--- a/Analysis/RandomForest/rf_test_plan_18042023.xlsx
+++ b/Analysis/RandomForest/rf_test_plan_18042023.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrismbrooks/Documents/Imperial/Asquith Group/KIR_HLA/Analysis/RandomForest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828DD37E-843C-FA45-A27D-CFBC34CFFD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B15E0B-E671-F54B-9C55-CDAB9E964872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="32140" windowHeight="17960" xr2:uid="{8A67EE38-8D0A-D541-B906-69B9E97D32A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Dataset</t>
   </si>
@@ -137,9 +137,6 @@
     <t>17042023_11</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>RF SS TrnTst MAE</t>
   </si>
   <si>
@@ -156,6 +153,12 @@
   </si>
   <si>
     <t>RF TrnTst MAE</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -163,10 +166,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -216,6 +219,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -253,8 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -275,23 +284,45 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA3A358-81BF-4F4F-9244-F1E6143260C2}">
-  <dimension ref="A3:S16"/>
+  <dimension ref="A3:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,783 +657,814 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3" t="s">
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="3" t="s">
+      <c r="L5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>36</v>
+      <c r="P5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7">
-        <v>300</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="J6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" s="7">
-        <v>200</v>
-      </c>
-      <c r="L6" s="13">
-        <v>-0.22094</v>
-      </c>
-      <c r="M6" s="8">
-        <f>($L$6-L6)/$L$6</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <v>100</v>
-      </c>
-      <c r="O6" s="7">
-        <v>6</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" s="8" t="e">
-        <f>($L$6-P6)/$L$6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="8" t="e">
-        <f>($L$6-R6)/$L$6</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="10">
+        <v>-0.22584199999999999</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="b">
+      <c r="C7" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="6" t="b">
+      <c r="E7" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
         <v>300</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>0.3</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>0.9</v>
       </c>
-      <c r="J7" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="7">
+      <c r="J7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
         <v>200</v>
       </c>
-      <c r="L7" s="15">
-        <v>-0.220945</v>
-      </c>
-      <c r="M7" s="8">
-        <f t="shared" ref="M7:M16" si="0">($L$6-L7)/$L$6</f>
-        <v>-2.2630578437607497E-5</v>
-      </c>
-      <c r="N7" s="7">
+      <c r="L7" s="8">
+        <v>-0.22094</v>
+      </c>
+      <c r="M7" s="7">
+        <f>($L$6-L7)/$L$6</f>
+        <v>2.1705440086432062E-2</v>
+      </c>
+      <c r="N7" s="6">
         <v>100</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="6">
         <v>6</v>
       </c>
-      <c r="P7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q7" s="8" t="e">
-        <f t="shared" ref="Q7:Q16" si="1">($L$6-P7)/$L$6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7" s="8" t="e">
-        <f t="shared" ref="S7:S16" si="2">($L$6-R7)/$L$6</f>
-        <v>#VALUE!</v>
+      <c r="P7" s="9">
+        <v>-0.207598139157011</v>
+      </c>
+      <c r="Q7" s="7">
+        <f>($L$6-P7)/$L$6</f>
+        <v>8.0781523556242796E-2</v>
+      </c>
+      <c r="R7" s="9">
+        <v>-0.20650388000987599</v>
+      </c>
+      <c r="S7" s="7">
+        <f>($L$6-R7)/$L$6</f>
+        <v>8.5626765571169217E-2</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="b">
+      <c r="C8" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="E8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
         <v>300</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>0.3</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>0.9</v>
       </c>
-      <c r="J8" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="J8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
         <v>200</v>
       </c>
-      <c r="L8" s="15">
-        <v>-0.220917</v>
-      </c>
-      <c r="M8" s="8">
-        <f t="shared" si="0"/>
-        <v>1.0410066081286886E-4</v>
-      </c>
-      <c r="N8" s="7">
+      <c r="L8" s="10">
+        <v>-0.220945</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" ref="M8:M17" si="0">($L$6-L8)/$L$6</f>
+        <v>2.1683300714658856E-2</v>
+      </c>
+      <c r="N8" s="6">
         <v>100</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="6">
         <v>6</v>
       </c>
-      <c r="P8" s="14">
-        <v>-0.20632468918696401</v>
-      </c>
-      <c r="Q8" s="8">
-        <f t="shared" si="1"/>
-        <v>6.6150587548818654E-2</v>
-      </c>
-      <c r="R8" s="14">
-        <v>-0.20108964985514699</v>
-      </c>
-      <c r="S8" s="8">
-        <f t="shared" si="2"/>
-        <v>8.9844981193324014E-2</v>
+      <c r="P8" s="9">
+        <v>-0.20815972268369101</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" ref="Q8:Q17" si="1">($L$6-P8)/$L$6</f>
+        <v>7.8294902260469604E-2</v>
+      </c>
+      <c r="R8" s="9">
+        <v>-0.20630779418496101</v>
+      </c>
+      <c r="S8" s="7">
+        <f t="shared" ref="S8:S17" si="2">($L$6-R8)/$L$6</f>
+        <v>8.6495008966618173E-2</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="E9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
         <v>300</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>0.3</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>0.9</v>
       </c>
-      <c r="J9" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="J9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6">
         <v>200</v>
       </c>
-      <c r="L9" s="15">
-        <v>-0.22059400000000001</v>
-      </c>
-      <c r="M9" s="8">
+      <c r="L9" s="10">
+        <v>-0.220917</v>
+      </c>
+      <c r="M9" s="7">
         <f t="shared" si="0"/>
-        <v>1.5660360278808058E-3</v>
-      </c>
-      <c r="N9" s="7">
+        <v>2.1807281196588701E-2</v>
+      </c>
+      <c r="N9" s="6">
         <v>100</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="6">
         <v>6</v>
       </c>
-      <c r="P9" s="14">
-        <v>-0.20982689980660199</v>
-      </c>
-      <c r="Q9" s="8">
+      <c r="P9" s="9">
+        <v>-0.20632468918696401</v>
+      </c>
+      <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>5.0299177122286626E-2</v>
-      </c>
-      <c r="R9" s="14">
-        <v>-0.209108085120084</v>
-      </c>
-      <c r="S9" s="8">
+        <v>8.6420200020527554E-2</v>
+      </c>
+      <c r="R9" s="9">
+        <v>-0.20108964985514699</v>
+      </c>
+      <c r="S9" s="7">
         <f t="shared" si="2"/>
-        <v>5.3552615551353308E-2</v>
+        <v>0.10960029642339776</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>300</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="J10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6">
+        <v>200</v>
+      </c>
+      <c r="L10" s="10">
+        <v>-0.22059400000000001</v>
+      </c>
+      <c r="M10" s="7">
+        <f t="shared" si="0"/>
+        <v>2.323748461313651E-2</v>
+      </c>
+      <c r="N10" s="6">
+        <v>100</v>
+      </c>
+      <c r="O10" s="6">
+        <v>6</v>
+      </c>
+      <c r="P10" s="9">
+        <v>-0.20982689980660199</v>
+      </c>
+      <c r="Q10" s="7">
+        <f t="shared" si="1"/>
+        <v>7.0912851433294066E-2</v>
+      </c>
+      <c r="R10" s="9">
+        <v>-0.209108085120084</v>
+      </c>
+      <c r="S10" s="7">
+        <f t="shared" si="2"/>
+        <v>7.409567254946374E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="E11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
         <v>300</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H11" s="6">
         <v>0.3</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I11" s="6">
         <v>0.9</v>
       </c>
-      <c r="J10" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10" s="7">
+      <c r="J11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
         <v>200</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L11" s="10">
         <v>-0.219834</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M11" s="7">
         <f t="shared" si="0"/>
-        <v>5.0058839503937533E-3</v>
-      </c>
-      <c r="N10" s="7">
+        <v>2.6602669122660912E-2</v>
+      </c>
+      <c r="N11" s="6">
         <v>100</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O11" s="6">
         <v>6</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P11" s="9">
         <v>-0.205635796746438</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q11" s="7">
         <f t="shared" si="1"/>
-        <v>6.9268594430895239E-2</v>
-      </c>
-      <c r="R10" s="14">
+        <v>8.9470529191036138E-2</v>
+      </c>
+      <c r="R11" s="9">
         <v>-0.19852006342285</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S11" s="7">
         <f t="shared" si="2"/>
-        <v>0.10147522665497419</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="11">
-        <v>300</v>
-      </c>
-      <c r="H11" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="I11" s="11">
-        <v>0.9</v>
-      </c>
-      <c r="J11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" s="11">
-        <v>200</v>
-      </c>
-      <c r="L11" s="15">
-        <v>-0.22048400000000001</v>
-      </c>
-      <c r="M11" s="8">
-        <f t="shared" si="0"/>
-        <v>2.0639087535076683E-3</v>
-      </c>
-      <c r="N11" s="11">
-        <v>100</v>
-      </c>
-      <c r="O11" s="11">
-        <v>6</v>
-      </c>
-      <c r="P11" s="14">
-        <v>-0.20632468918696401</v>
-      </c>
-      <c r="Q11" s="8">
-        <f t="shared" si="1"/>
-        <v>6.6150587548818654E-2</v>
-      </c>
-      <c r="R11" s="14">
-        <v>-0.20108964985514699</v>
-      </c>
-      <c r="S11" s="8">
-        <f t="shared" si="2"/>
-        <v>8.9844981193324014E-2</v>
+        <v>0.12097810228898959</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>300</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="J12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <v>200</v>
+      </c>
+      <c r="L12" s="10">
+        <v>-0.22048400000000001</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" si="0"/>
+        <v>2.3724550792146609E-2</v>
+      </c>
+      <c r="N12" s="6">
+        <v>100</v>
+      </c>
+      <c r="O12" s="6">
+        <v>6</v>
+      </c>
+      <c r="P12" s="9">
+        <v>-0.20632468918696401</v>
+      </c>
+      <c r="Q12" s="7">
+        <f t="shared" si="1"/>
+        <v>8.6420200020527554E-2</v>
+      </c>
+      <c r="R12" s="9">
+        <v>-0.20108964985514699</v>
+      </c>
+      <c r="S12" s="7">
+        <f t="shared" si="2"/>
+        <v>0.10960029642339776</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="b">
+      <c r="C13" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="E13" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="18">
         <v>300</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="18">
         <v>0.3</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I13" s="18">
         <v>0.9</v>
       </c>
-      <c r="J12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="7">
+      <c r="J13" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="18">
         <v>200</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L13" s="19">
         <v>-0.22017400000000001</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M13" s="20">
         <f t="shared" si="0"/>
-        <v>3.4670046166379513E-3</v>
-      </c>
-      <c r="N12" s="7">
+        <v>2.5097191842084195E-2</v>
+      </c>
+      <c r="N13" s="18">
         <v>100</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O13" s="18">
         <v>6</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P13" s="21">
         <v>-0.20571772967930299</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="Q13" s="20">
         <f t="shared" si="1"/>
-        <v>6.8897756498130749E-2</v>
-      </c>
-      <c r="R12" s="14">
+        <v>8.9107740458803042E-2</v>
+      </c>
+      <c r="R13" s="21">
         <v>-0.19480828159764099</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S13" s="20">
         <f t="shared" si="2"/>
-        <v>0.11827518060269307</v>
+        <v>0.13741340584284145</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="E14" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
         <v>300</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H14" s="6">
         <v>0.3</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I14" s="6">
         <v>0.9</v>
       </c>
-      <c r="J13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="J14" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6">
         <v>200</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L14" s="10">
         <v>-0.219748</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M14" s="7">
         <f t="shared" si="0"/>
-        <v>5.3951298995202259E-3</v>
-      </c>
-      <c r="N13" s="7">
+        <v>2.6983466317159734E-2</v>
+      </c>
+      <c r="N14" s="6">
         <v>100</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O14" s="6">
         <v>6</v>
       </c>
-      <c r="P13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q13" s="8" t="e">
+      <c r="P14" s="9">
+        <v>-0.20646087192420801</v>
+      </c>
+      <c r="Q14" s="7">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R13" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="S13" s="8" t="e">
+        <v>8.5817199970740526E-2</v>
+      </c>
+      <c r="R14" s="9">
+        <v>-0.204141952142987</v>
+      </c>
+      <c r="S14" s="7">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>9.6085085400470199E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+    <row r="15" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="11">
+      <c r="E15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="18">
         <v>300</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H15" s="18">
         <v>0.3</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I15" s="18">
         <v>0.9</v>
       </c>
-      <c r="J14" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="J15" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="18">
         <v>200</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L15" s="19">
         <v>-0.21963099999999999</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M15" s="20">
         <f t="shared" si="0"/>
-        <v>5.9246854349597382E-3</v>
-      </c>
-      <c r="N14" s="11">
+        <v>2.7501527616652328E-2</v>
+      </c>
+      <c r="N15" s="18">
         <v>100</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O15" s="18">
         <v>6</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P15" s="21">
         <v>-0.20513934215975499</v>
       </c>
-      <c r="Q14" s="8">
+      <c r="Q15" s="20">
         <f t="shared" si="1"/>
-        <v>7.151560532382098E-2</v>
-      </c>
-      <c r="R14" s="14">
+        <v>9.1668767723651928E-2</v>
+      </c>
+      <c r="R15" s="21">
         <v>-0.19685328328648799</v>
       </c>
-      <c r="S14" s="8">
+      <c r="S15" s="20">
         <f t="shared" si="2"/>
-        <v>0.10901926637780396</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="7">
-        <v>300</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I15" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="J15" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="7">
-        <v>200</v>
-      </c>
-      <c r="L15" s="15">
-        <v>-0.22018199999999999</v>
-      </c>
-      <c r="M15" s="8">
-        <f t="shared" si="0"/>
-        <v>3.4307956911379047E-3</v>
-      </c>
-      <c r="N15" s="7">
-        <v>100</v>
-      </c>
-      <c r="O15" s="7">
-        <v>6</v>
-      </c>
-      <c r="P15" s="14">
-        <v>-0.20613035087505599</v>
-      </c>
-      <c r="Q15" s="8">
-        <f t="shared" si="1"/>
-        <v>6.7030185231031089E-2</v>
-      </c>
-      <c r="R15" s="14">
-        <v>-0.20072957628139601</v>
-      </c>
-      <c r="S15" s="8">
-        <f t="shared" si="2"/>
-        <v>9.1474715844138618E-2</v>
+        <v>0.12835839530960583</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>300</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="J16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="6">
+        <v>200</v>
+      </c>
+      <c r="L16" s="10">
+        <v>-0.22018199999999999</v>
+      </c>
+      <c r="M16" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5061768847247184E-2</v>
+      </c>
+      <c r="N16" s="6">
+        <v>100</v>
+      </c>
+      <c r="O16" s="6">
+        <v>6</v>
+      </c>
+      <c r="P16" s="9">
+        <v>-0.20613035087505599</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" si="1"/>
+        <v>8.7280705647948556E-2</v>
+      </c>
+      <c r="R16" s="9">
+        <v>-0.20072957628139601</v>
+      </c>
+      <c r="S16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.11119465696639233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="6" t="b">
+      <c r="C17" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7">
+      <c r="E17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
         <v>300</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H17" s="6">
         <v>0.3</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I17" s="6">
         <v>0.9</v>
       </c>
-      <c r="J16" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" s="7">
+      <c r="J17" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="6">
         <v>200</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L17" s="10">
         <v>-0.219496</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M17" s="7">
         <f t="shared" si="0"/>
-        <v>6.5357110527745127E-3</v>
-      </c>
-      <c r="N16" s="7">
+        <v>2.8099290654528347E-2</v>
+      </c>
+      <c r="N17" s="6">
         <v>100</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O17" s="6">
         <v>6</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P17" s="9">
         <v>-0.206530224991512</v>
       </c>
-      <c r="Q16" s="8">
+      <c r="Q17" s="7">
         <f t="shared" si="1"/>
-        <v>6.5220308719507569E-2</v>
-      </c>
-      <c r="R16" s="14">
+        <v>8.5510113302609755E-2</v>
+      </c>
+      <c r="R17" s="9">
         <v>-0.203735728630484</v>
       </c>
-      <c r="S16" s="8">
+      <c r="S17" s="7">
         <f t="shared" si="2"/>
-        <v>7.7868522537865456E-2</v>
+        <v>9.7883792073732892E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="M6:S6"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>

</xml_diff>

<commit_message>
Big Blunder But Hopefully its All Fixed Now
</commit_message>
<xml_diff>
--- a/Analysis/RandomForest/rf_test_plan_18042023.xlsx
+++ b/Analysis/RandomForest/rf_test_plan_18042023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrismbrooks/Documents/Imperial/Asquith Group/KIR_HLA/Analysis/RandomForest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B15E0B-E671-F54B-9C55-CDAB9E964872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1D0240-CEE1-C642-A9E1-CBD43EB6B769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="500" windowWidth="32140" windowHeight="17960" xr2:uid="{8A67EE38-8D0A-D541-B906-69B9E97D32A4}"/>
+    <workbookView xWindow="820" yWindow="5100" windowWidth="31980" windowHeight="18440" xr2:uid="{8A67EE38-8D0A-D541-B906-69B9E97D32A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,36 +293,41 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +646,7 @@
   <dimension ref="A3:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,27 +662,27 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="21" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="21" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="1"/>
@@ -705,13 +710,13 @@
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
@@ -751,33 +756,33 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
       <c r="L6" s="10">
         <v>-0.22584199999999999</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -958,11 +963,11 @@
         <v>8.6420200020527554E-2</v>
       </c>
       <c r="R9" s="9">
-        <v>-0.20108964985514699</v>
+        <v>-0.20534123008563199</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="2"/>
-        <v>0.10960029642339776</v>
+        <v>9.077483335415025E-2</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1020,11 +1025,11 @@
         <v>7.0912851433294066E-2</v>
       </c>
       <c r="R10" s="9">
-        <v>-0.209108085120084</v>
+        <v>-0.210379915108865</v>
       </c>
       <c r="S10" s="7">
         <f t="shared" si="2"/>
-        <v>7.409567254946374E-2</v>
+        <v>6.846416915868167E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -1082,11 +1087,11 @@
         <v>8.9470529191036138E-2</v>
       </c>
       <c r="R11" s="9">
-        <v>-0.19852006342285</v>
+        <v>-0.20403784380727999</v>
       </c>
       <c r="S11" s="7">
         <f t="shared" si="2"/>
-        <v>0.12097810228898959</v>
+        <v>9.6546064030251233E-2</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1144,73 +1149,73 @@
         <v>8.6420200020527554E-2</v>
       </c>
       <c r="R12" s="9">
-        <v>-0.20108964985514699</v>
+        <v>-0.20534123008563199</v>
       </c>
       <c r="S12" s="7">
         <f t="shared" si="2"/>
-        <v>0.10960029642339776</v>
+        <v>9.077483335415025E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="17" t="b">
+      <c r="C13" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="18">
+      <c r="E13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
         <v>300</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="13">
         <v>0.3</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="13">
         <v>0.9</v>
       </c>
-      <c r="J13" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="18">
+      <c r="J13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="13">
         <v>200</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13" s="14">
         <v>-0.22017400000000001</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="15">
         <f t="shared" si="0"/>
         <v>2.5097191842084195E-2</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="13">
         <v>100</v>
       </c>
-      <c r="O13" s="18">
+      <c r="O13" s="13">
         <v>6</v>
       </c>
-      <c r="P13" s="21">
+      <c r="P13" s="16">
         <v>-0.20571772967930299</v>
       </c>
-      <c r="Q13" s="20">
+      <c r="Q13" s="15">
         <f t="shared" si="1"/>
         <v>8.9107740458803042E-2</v>
       </c>
-      <c r="R13" s="21">
-        <v>-0.19480828159764099</v>
-      </c>
-      <c r="S13" s="20">
+      <c r="R13" s="16">
+        <v>-0.20194184251116901</v>
+      </c>
+      <c r="S13" s="15">
         <f t="shared" si="2"/>
-        <v>0.13741340584284145</v>
+        <v>0.10582689441658763</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -1275,66 +1280,66 @@
         <v>9.6085085400470199E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="18">
+      <c r="E15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="23">
         <v>300</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="23">
         <v>0.3</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="23">
         <v>0.9</v>
       </c>
-      <c r="J15" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="18">
+      <c r="J15" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="23">
         <v>200</v>
       </c>
-      <c r="L15" s="19">
+      <c r="L15" s="10">
         <v>-0.21963099999999999</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="24">
         <f t="shared" si="0"/>
         <v>2.7501527616652328E-2</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="23">
         <v>100</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="23">
         <v>6</v>
       </c>
-      <c r="P15" s="21">
+      <c r="P15" s="9">
         <v>-0.20513934215975499</v>
       </c>
-      <c r="Q15" s="20">
+      <c r="Q15" s="24">
         <f t="shared" si="1"/>
         <v>9.1668767723651928E-2</v>
       </c>
-      <c r="R15" s="21">
-        <v>-0.19685328328648799</v>
-      </c>
-      <c r="S15" s="20">
+      <c r="R15" s="9">
+        <v>-0.20475599365028699</v>
+      </c>
+      <c r="S15" s="24">
         <f t="shared" si="2"/>
-        <v>0.12835839530960583</v>
+        <v>9.3366186757613726E-2</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1392,11 +1397,11 @@
         <v>8.7280705647948556E-2</v>
       </c>
       <c r="R16" s="9">
-        <v>-0.20072957628139601</v>
+        <v>-0.204048554758305</v>
       </c>
       <c r="S16" s="7">
         <f t="shared" si="2"/>
-        <v>0.11119465696639233</v>
+        <v>9.6498637284893829E-2</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
@@ -1454,11 +1459,11 @@
         <v>8.5510113302609755E-2</v>
       </c>
       <c r="R17" s="9">
-        <v>-0.203735728630484</v>
+        <v>-0.20485890442044699</v>
       </c>
       <c r="S17" s="7">
         <f t="shared" si="2"/>
-        <v>9.7883792073732892E-2</v>
+        <v>9.2910510797606274E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>